<commit_message>
Finished TMD model code
Used capacitor, Vth model to figure out N
</commit_message>
<xml_diff>
--- a/tmd-javey-plqy.xlsx
+++ b/tmd-javey-plqy.xlsx
@@ -8,14 +8,23 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/corawent/Documents/GitHub/tmd-model/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4E8967A5-2305-8D4B-8B3F-0569706AE5B1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{040DB8F1-DD23-FE4B-BD3D-EC8DDAFB1C5B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="80" yWindow="460" windowWidth="25440" windowHeight="14720" activeTab="1" xr2:uid="{D1C0AD63-CF25-AE4D-AB39-12D67C4E5330}"/>
+    <workbookView xWindow="80" yWindow="460" windowWidth="25440" windowHeight="14720" activeTab="6" xr2:uid="{D1C0AD63-CF25-AE4D-AB39-12D67C4E5330}"/>
   </bookViews>
   <sheets>
-    <sheet name="MoS2_-20V" sheetId="1" r:id="rId1"/>
-    <sheet name="MoS2_0V" sheetId="2" r:id="rId2"/>
-    <sheet name="MoS2_20V" sheetId="3" r:id="rId3"/>
+    <sheet name="MoS_2_-20V" sheetId="1" r:id="rId1"/>
+    <sheet name="MoS_2_0V" sheetId="2" r:id="rId2"/>
+    <sheet name="MoS_2_20V" sheetId="3" r:id="rId3"/>
+    <sheet name="WS_2_-20V" sheetId="7" r:id="rId4"/>
+    <sheet name="WS_2_0V" sheetId="8" r:id="rId5"/>
+    <sheet name="WS_2_20V" sheetId="9" r:id="rId6"/>
+    <sheet name="MoSe_2_-20V" sheetId="10" r:id="rId7"/>
+    <sheet name="MoSe_2_-5V" sheetId="11" r:id="rId8"/>
+    <sheet name="MoSe_2_20V" sheetId="12" r:id="rId9"/>
+    <sheet name="WSe_2_-20V" sheetId="6" r:id="rId10"/>
+    <sheet name="WSe_2_0V" sheetId="4" r:id="rId11"/>
+    <sheet name="WSe_2_20V" sheetId="5" r:id="rId12"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -27,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="2">
   <si>
     <t>G</t>
   </si>
@@ -71,8 +80,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -391,7 +401,7 @@
   <dimension ref="A1:B18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B18"/>
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -408,139 +418,584 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="2">
+        <v>1019084463595530</v>
+      </c>
+      <c r="B2" s="2">
+        <v>83.693796144374204</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="2">
+        <v>3216541525900940</v>
+      </c>
+      <c r="B3" s="2">
+        <v>72.919367470397304</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="2">
+        <v>6257307826894880</v>
+      </c>
+      <c r="B4" s="2">
+        <v>72.919367470397304</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="2">
+        <v>1.21726708407884E+16</v>
+      </c>
+      <c r="B5" s="2">
+        <v>76.347183005999398</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="2">
+        <v>3.10892923951884E+16</v>
+      </c>
+      <c r="B6" s="2">
+        <v>49.3476905756037</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="2">
+        <v>6.0479639721905E+16</v>
+      </c>
+      <c r="B7" s="2">
+        <v>40.132043269401102</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" s="2">
+        <v>1.2126733747095E+17</v>
+      </c>
+      <c r="B8" s="2">
+        <v>31.896325041280999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="2">
+        <v>3.0971967959466803E+17</v>
+      </c>
+      <c r="B9" s="2">
+        <v>19.690844346458501</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" s="2">
+        <v>6.0251402311003597E+17</v>
+      </c>
+      <c r="B10" s="2">
+        <v>12.438359139222101</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" s="2">
+        <v>1.2080970010309299E+18</v>
+      </c>
+      <c r="B11" s="2">
+        <v>7.85709212637689</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" s="2">
+        <v>3.0855086281432699E+18</v>
+      </c>
+      <c r="B12" s="2">
+        <v>4.7403507113052399</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" s="2">
+        <v>6.3767251903232799E+18</v>
+      </c>
+      <c r="B13" s="2">
+        <v>3.0639684518936501</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" s="2">
+        <v>1.27859307557079E+19</v>
+      </c>
+      <c r="B14" s="2">
+        <v>1.89150711847255</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" s="2">
+        <v>2.9822801650712199E+19</v>
+      </c>
+      <c r="B15" s="2">
+        <v>0.94963368149654404</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" s="2">
+        <v>5.9797508198387704E+19</v>
+      </c>
+      <c r="B16" s="2">
+        <v>0.599866850467493</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" s="2">
+        <v>1.2358165955824199E+20</v>
+      </c>
+      <c r="B17" s="2">
+        <v>0.378925311202855</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" s="2">
+        <v>3.3531390233288999E+20</v>
+      </c>
+      <c r="B18" s="2">
+        <v>0.19466003986510799</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACFD8C0E-DFA0-6146-AC7B-E85EA943C810}">
+  <dimension ref="A1:B17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
-        <v>1019084463595530</v>
+        <v>994150000000000</v>
       </c>
       <c r="B2" s="1">
-        <v>83.693796144374204</v>
+        <v>1.4873499999999999</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
-        <v>3216541525900940</v>
+        <v>1.55175E+16</v>
       </c>
       <c r="B3" s="1">
-        <v>72.919367470397304</v>
+        <v>1.18249</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
-        <v>6257307826894880</v>
+        <v>3.53939E+16</v>
       </c>
       <c r="B4" s="1">
-        <v>72.919367470397304</v>
+        <v>1.1414899999999999</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
-        <v>1.21726708407884E+16</v>
+        <v>7.59988E+16</v>
       </c>
       <c r="B5" s="1">
-        <v>76.347183005999398</v>
+        <v>1.22496</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
-        <v>3.10892923951884E+16</v>
+        <v>1.53569E+17</v>
       </c>
       <c r="B6" s="1">
-        <v>49.3476905756037</v>
+        <v>1.3859999999999999</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
-        <v>6.0479639721905E+16</v>
+        <v>3.00871E+17</v>
       </c>
       <c r="B7" s="1">
-        <v>40.132043269401102</v>
+        <v>1.4873499999999999</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
-        <v>1.2126733747095E+17</v>
+        <v>6.26309E+17</v>
       </c>
       <c r="B8" s="1">
-        <v>31.896325041280999</v>
+        <v>1.4873499999999999</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
-        <v>3.0971967959466803E+17</v>
+        <v>1.77205E+18</v>
       </c>
       <c r="B9" s="1">
-        <v>19.690844346458501</v>
+        <v>1.83809</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
-        <v>6.0251402311003597E+17</v>
+        <v>3.1711E+18</v>
       </c>
       <c r="B10" s="1">
-        <v>12.438359139222101</v>
+        <v>2.3119800000000001</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
-        <v>1.2080970010309299E+18</v>
+        <v>6.6135E+18</v>
       </c>
       <c r="B11" s="1">
-        <v>7.85709212637689</v>
+        <v>3.0661299999999998</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
-        <v>3.0855086281432699E+18</v>
+        <v>1.60408E+19</v>
       </c>
       <c r="B12" s="1">
-        <v>4.7403507113052399</v>
+        <v>3.1207099999999999</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
-        <v>6.3767251903232799E+18</v>
+        <v>3.04422E+19</v>
       </c>
       <c r="B13" s="1">
-        <v>3.0639684518936501</v>
+        <v>2.7581199999999999</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
-        <v>1.27859307557079E+19</v>
+        <v>6.53359E+19</v>
       </c>
       <c r="B14" s="1">
-        <v>1.89150711847255</v>
+        <v>2.7581199999999999</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
-        <v>2.9822801650712199E+19</v>
+        <v>1.73252E+20</v>
       </c>
       <c r="B15" s="1">
-        <v>0.94963368149654404</v>
+        <v>1.93801</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
-        <v>5.9797508198387704E+19</v>
+        <v>3.09058E+20</v>
       </c>
       <c r="B16" s="1">
-        <v>0.599866850467493</v>
+        <v>1.51383</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
-        <v>1.2358165955824199E+20</v>
+        <v>5.6841900000000003E+20</v>
       </c>
       <c r="B17" s="1">
-        <v>0.378925311202855</v>
+        <v>1.18249</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10E9E812-4257-BF4B-9B3C-2FF8B326B10A}">
+  <dimension ref="A1:B19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="1">
+        <v>1100590000000000</v>
+      </c>
+      <c r="B2" s="1">
+        <v>6.7829300000000003</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="1">
+        <v>4090730000000000</v>
+      </c>
+      <c r="B3" s="1">
+        <v>6.1015600000000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
+        <v>6875250000000000</v>
+      </c>
+      <c r="B4" s="1">
+        <v>5.9948399999999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
+        <v>1.61872E+16</v>
+      </c>
+      <c r="B5" s="1">
+        <v>6.9036799999999996</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
+        <v>3.58232E+16</v>
+      </c>
+      <c r="B6" s="1">
+        <v>7.0265700000000004</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="1">
+        <v>7.45626E+16</v>
+      </c>
+      <c r="B7" s="1">
+        <v>6.9036799999999996</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" s="1">
+        <v>1.60103E+17</v>
+      </c>
+      <c r="B8" s="1">
+        <v>7.4085299999999998</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="1">
+        <v>3.04164E+17</v>
+      </c>
+      <c r="B9" s="1">
+        <v>7.6746299999999996</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" s="1">
+        <v>6.72188E+17</v>
+      </c>
+      <c r="B10" s="1">
+        <v>6.3207199999999997</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" s="1">
+        <v>1.786E+18</v>
+      </c>
+      <c r="B11" s="1">
+        <v>5.9948399999999999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" s="1">
+        <v>3.18748E+18</v>
+      </c>
+      <c r="B12" s="1">
+        <v>5.02515</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" s="1">
+        <v>6.63211E+18</v>
+      </c>
+      <c r="B13" s="1">
+        <v>4.6827199999999998</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" s="1">
+        <v>1.5591E+19</v>
+      </c>
+      <c r="B14" s="1">
+        <v>4.2873000000000001</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" s="1">
+        <v>3.14491E+19</v>
+      </c>
+      <c r="B15" s="1">
+        <v>3.7229000000000001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" s="1">
+        <v>6.52518E+19</v>
+      </c>
+      <c r="B16" s="1">
+        <v>2.27155</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" s="1">
+        <v>1.7305E+20</v>
+      </c>
+      <c r="B17" s="1">
+        <v>1.62453</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
-        <v>3.3531390233288999E+20</v>
+        <v>3.1823500000000003E+20</v>
       </c>
       <c r="B18" s="1">
-        <v>0.19466003986510799</v>
+        <v>1.2467699999999999</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" s="1">
+        <v>5.67688E+20</v>
+      </c>
+      <c r="B19" s="1">
+        <v>0.973881</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55725661-D964-0D48-8C0F-938A90869228}">
+  <dimension ref="A1:B14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H20" sqref="H20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="1">
+        <v>973881000000000</v>
+      </c>
+      <c r="B2" s="1">
+        <v>6.6642999999999994E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="1">
+        <v>1.55504E+17</v>
+      </c>
+      <c r="B3" s="1">
+        <v>9.1555800000000007E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
+        <v>3.04307E+17</v>
+      </c>
+      <c r="B4" s="1">
+        <v>8.2358600000000004E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
+        <v>6.3346E+17</v>
+      </c>
+      <c r="B5" s="1">
+        <v>8.2358600000000004E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
+        <v>1.58316E+18</v>
+      </c>
+      <c r="B6" s="1">
+        <v>7.6746300000000003E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="1">
+        <v>3.50404E+18</v>
+      </c>
+      <c r="B7" s="1">
+        <v>7.9502900000000001E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" s="1">
+        <v>7.07474E+18</v>
+      </c>
+      <c r="B8" s="1">
+        <v>7.9502900000000001E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="1">
+        <v>1.56403E+19</v>
+      </c>
+      <c r="B9" s="1">
+        <v>6.9036799999999995E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" s="1">
+        <v>2.97031E+19</v>
+      </c>
+      <c r="B10" s="1">
+        <v>6.7829299999999995E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" s="1">
+        <v>6.18605E+19</v>
+      </c>
+      <c r="B11" s="1">
+        <v>7.2789499999999993E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" s="1">
+        <v>1.69402E+20</v>
+      </c>
+      <c r="B12" s="1">
+        <v>6.5477499999999994E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" s="1">
+        <v>3.31736E+20</v>
+      </c>
+      <c r="B13" s="1">
+        <v>6.5477499999999994E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" s="1">
+        <v>5.40962E+20</v>
+      </c>
+      <c r="B14" s="1">
+        <v>6.7829299999999995E-2</v>
       </c>
     </row>
   </sheetData>
@@ -552,8 +1007,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4ADAC824-AFE4-304C-B1B0-962DF684E76C}">
   <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -571,90 +1026,90 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="1">
+      <c r="A2" s="2">
         <v>1019080000000000</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2" s="2">
         <v>7.5910000000000005E-2</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="1">
+      <c r="A3" s="2">
         <v>1.24991E+17</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B3" s="2">
         <v>0.122963</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" s="1">
+      <c r="A4" s="2">
         <v>3.0972E+17</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B4" s="2">
         <v>0.104701</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="1">
+      <c r="A5" s="2">
         <v>6.02514E+17</v>
       </c>
-      <c r="B5" s="1">
+      <c r="B5" s="2">
         <v>0.1</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" s="1">
+      <c r="A6" s="2">
         <v>1.2081E+18</v>
       </c>
-      <c r="B6" s="1">
+      <c r="B6" s="2">
         <v>9.3341499999999994E-2</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" s="1">
+      <c r="A7" s="2">
         <v>2.90439E+18</v>
       </c>
-      <c r="B7" s="1">
+      <c r="B7" s="2">
         <v>8.7126400000000007E-2</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" s="1">
+      <c r="A8" s="2">
         <v>6.0024E+18</v>
       </c>
-      <c r="B8" s="1">
+      <c r="B8" s="2">
         <v>7.9478400000000005E-2</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" s="1">
+      <c r="A9" s="2">
         <v>1.2405E+19</v>
       </c>
-      <c r="B9" s="1">
+      <c r="B9" s="2">
         <v>7.41864E-2</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" s="1">
+      <c r="A10" s="2">
         <v>2.98228E+19</v>
       </c>
-      <c r="B10" s="1">
+      <c r="B10" s="2">
         <v>6.6137699999999994E-2</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11" s="1">
+      <c r="A11" s="2">
         <v>6.16339E+19</v>
       </c>
-      <c r="B11" s="1">
+      <c r="B11" s="2">
         <v>6.6137699999999994E-2</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12" s="1">
+      <c r="A12" s="2">
         <v>1.199E+20</v>
       </c>
-      <c r="B12" s="1">
+      <c r="B12" s="2">
         <v>5.50362E-2</v>
       </c>
     </row>
@@ -668,7 +1123,7 @@
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -686,83 +1141,917 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="2">
+        <v>1019080000000000</v>
+      </c>
+      <c r="B2" s="2">
+        <v>5.2565199999999999E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="2">
+        <v>6.21017E+17</v>
+      </c>
+      <c r="B3" s="2">
+        <v>6.9246699999999994E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="2">
+        <v>1.28344E+18</v>
+      </c>
+      <c r="B4" s="2">
+        <v>6.03321E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="2">
+        <v>2.99358E+18</v>
+      </c>
+      <c r="B5" s="2">
+        <v>5.3786500000000001E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="2">
+        <v>6.18673E+18</v>
+      </c>
+      <c r="B6" s="2">
+        <v>5.50362E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="2">
+        <v>1.2405E+19</v>
+      </c>
+      <c r="B7" s="2">
+        <v>4.7951000000000001E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" s="2">
+        <v>3.07386E+19</v>
+      </c>
+      <c r="B8" s="2">
+        <v>4.5798100000000001E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="2">
+        <v>6.54775E+19</v>
+      </c>
+      <c r="B9" s="2">
+        <v>4.37419E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" s="2">
+        <v>1.199E+20</v>
+      </c>
+      <c r="B10" s="2">
+        <v>4.4758199999999998E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" s="2">
+        <v>3.2532300000000003E+20</v>
+      </c>
+      <c r="B11" s="2">
+        <v>3.8110699999999997E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28DACF07-9399-DA48-876B-5EA42D57E5C5}">
+  <dimension ref="A1:B18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I19" sqref="I19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
-        <v>1019080000000000</v>
+        <v>962473000000000</v>
       </c>
       <c r="B2" s="1">
-        <v>5.2565199999999999E-2</v>
+        <v>69.131600000000006</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
-        <v>6.21017E+17</v>
+        <v>2724060000000000</v>
       </c>
       <c r="B3" s="1">
-        <v>6.9246699999999994E-2</v>
+        <v>80.669700000000006</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
-        <v>1.28344E+18</v>
+        <v>5506350000000000</v>
       </c>
       <c r="B4" s="1">
-        <v>6.03321E-2</v>
+        <v>71.739000000000004</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
-        <v>2.99358E+18</v>
+        <v>1.0795E+16</v>
       </c>
       <c r="B5" s="1">
-        <v>5.3786500000000001E-2</v>
+        <v>88.771500000000003</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
-        <v>6.18673E+18</v>
+        <v>2.54282E+16</v>
       </c>
       <c r="B6" s="1">
-        <v>5.50362E-2</v>
+        <v>86.9846</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
-        <v>1.2405E+19</v>
+        <v>5.98975E+16</v>
       </c>
       <c r="B7" s="1">
-        <v>4.7951000000000001E-2</v>
+        <v>80.4071</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
-        <v>3.07386E+19</v>
+        <v>1.21076E+17</v>
       </c>
       <c r="B8" s="1">
-        <v>4.5798100000000001E-2</v>
+        <v>71.505499999999998</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
-        <v>6.54775E+19</v>
+        <v>3.1262E+17</v>
       </c>
       <c r="B9" s="1">
-        <v>4.37419E-2</v>
+        <v>56.576900000000002</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
-        <v>1.199E+20</v>
+        <v>6.1288E+17</v>
       </c>
       <c r="B10" s="1">
-        <v>4.4758199999999998E-2</v>
+        <v>37.593699999999998</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
-        <v>3.2532300000000003E+20</v>
+        <v>1.58247E+18</v>
       </c>
       <c r="B11" s="1">
-        <v>3.8110699999999997E-2</v>
+        <v>32.1492</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" s="1">
+        <v>3.10238E+18</v>
+      </c>
+      <c r="B12" s="1">
+        <v>22.2088</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" s="1">
+        <v>6.46593E+18</v>
+      </c>
+      <c r="B13" s="1">
+        <v>16.906099999999999</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" s="1">
+        <v>1.30701E+19</v>
+      </c>
+      <c r="B14" s="1">
+        <v>11.6784</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" s="1">
+        <v>3.1744E+19</v>
+      </c>
+      <c r="B15" s="1">
+        <v>6.5134800000000004</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" s="1">
+        <v>6.22329E+19</v>
+      </c>
+      <c r="B16" s="1">
+        <v>5.2562699999999998</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" s="1">
+        <v>1.25796E+20</v>
+      </c>
+      <c r="B17" s="1">
+        <v>3.4925299999999999</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" s="1">
+        <v>2.18208E+20</v>
+      </c>
+      <c r="B18" s="1">
+        <v>2.8740899999999998</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E760E4E-8171-944E-908F-FE48C83C7AA0}">
+  <dimension ref="A1:B16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:B16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="1">
+        <v>1087790000000000</v>
+      </c>
+      <c r="B2" s="1">
+        <v>1.33826</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="1">
+        <v>1.04697E+16</v>
+      </c>
+      <c r="B3" s="1">
+        <v>2.1283099999999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
+        <v>2.54282E+16</v>
+      </c>
+      <c r="B4" s="1">
+        <v>1.7851699999999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
+        <v>6.17586E+16</v>
+      </c>
+      <c r="B5" s="1">
+        <v>1.8184899999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
+        <v>1.24838E+17</v>
+      </c>
+      <c r="B6" s="1">
+        <v>1.6812499999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="1">
+        <v>3.22334E+17</v>
+      </c>
+      <c r="B7" s="1">
+        <v>1.58446</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" s="1">
+        <v>6.1288E+17</v>
+      </c>
+      <c r="B8" s="1">
+        <v>1.3037700000000001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="1">
+        <v>1.63164E+18</v>
+      </c>
+      <c r="B9" s="1">
+        <v>1.2286699999999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" s="1">
+        <v>3.19877E+18</v>
+      </c>
+      <c r="B10" s="1">
+        <v>1.2764500000000001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" s="1">
+        <v>6.27108E+18</v>
+      </c>
+      <c r="B11" s="1">
+        <v>1.2755399999999999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" s="1">
+        <v>1.26762E+19</v>
+      </c>
+      <c r="B12" s="1">
+        <v>1.2746</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" s="1">
+        <v>3.1744E+19</v>
+      </c>
+      <c r="B13" s="1">
+        <v>1.2488600000000001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" s="1">
+        <v>6.22329E+19</v>
+      </c>
+      <c r="B14" s="1">
+        <v>1.1106400000000001</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" s="1">
+        <v>1.29705E+20</v>
+      </c>
+      <c r="B15" s="1">
+        <v>0.96864399999999995</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" s="1">
+        <v>2.24988E+20</v>
+      </c>
+      <c r="B16" s="1">
+        <v>0.94945199999999996</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2D2F849-FD11-6946-9633-185FCE7AF0F9}">
+  <dimension ref="A1:B15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J28" sqref="J28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="1">
+        <v>992379000000000</v>
+      </c>
+      <c r="B2" s="1">
+        <v>0.53698000000000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="1">
+        <v>2.62183E+16</v>
+      </c>
+      <c r="B3" s="1">
+        <v>0.61309800000000003</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
+        <v>5.80924E+16</v>
+      </c>
+      <c r="B4" s="1">
+        <v>0.60079499999999997</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
+        <v>1.32716E+17</v>
+      </c>
+      <c r="B5" s="1">
+        <v>0.54469500000000004</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
+        <v>3.1262E+17</v>
+      </c>
+      <c r="B6" s="1">
+        <v>0.56576899999999997</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="1">
+        <v>6.51559E+17</v>
+      </c>
+      <c r="B7" s="1">
+        <v>0.50311799999999995</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" s="1">
+        <v>1.53478E+18</v>
+      </c>
+      <c r="B8" s="1">
+        <v>0.42201499999999997</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="1">
+        <v>3.10238E+18</v>
+      </c>
+      <c r="B9" s="1">
+        <v>0.464729</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" s="1">
+        <v>6.46593E+18</v>
+      </c>
+      <c r="B10" s="1">
+        <v>0.51174900000000001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" s="1">
+        <v>1.26762E+19</v>
+      </c>
+      <c r="B11" s="1">
+        <v>0.48242800000000002</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" s="1">
+        <v>3.1744E+19</v>
+      </c>
+      <c r="B12" s="1">
+        <v>0.51089099999999998</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" s="1">
+        <v>6.41666E+19</v>
+      </c>
+      <c r="B13" s="1">
+        <v>0.44558799999999998</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" s="1">
+        <v>1.25796E+20</v>
+      </c>
+      <c r="B14" s="1">
+        <v>0.42830000000000001</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" s="1">
+        <v>2.31979E+20</v>
+      </c>
+      <c r="B15" s="1">
+        <v>0.44498500000000002</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36E34563-729E-9B4D-A695-9565F3F4FE9B}">
+  <dimension ref="A1:B15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:B15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="1">
+        <v>1008350000000000</v>
+      </c>
+      <c r="B2" s="1">
+        <v>0.39626899999999998</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="1">
+        <v>4.04109E+16</v>
+      </c>
+      <c r="B3" s="1">
+        <v>0.38720399999999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
+        <v>6.22621E+16</v>
+      </c>
+      <c r="B4" s="1">
+        <v>0.32176399999999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
+        <v>1.86534E+17</v>
+      </c>
+      <c r="B5" s="1">
+        <v>0.30018400000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
+        <v>3.62716E+17</v>
+      </c>
+      <c r="B6" s="1">
+        <v>0.23816899999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="1">
+        <v>6.82237E+17</v>
+      </c>
+      <c r="B7" s="1">
+        <v>0.24945100000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" s="1">
+        <v>1.61952E+18</v>
+      </c>
+      <c r="B8" s="1">
+        <v>0.19338900000000001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="1">
+        <v>3.3657E+18</v>
+      </c>
+      <c r="B9" s="1">
+        <v>0.217112</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" s="1">
+        <v>6.12355E+18</v>
+      </c>
+      <c r="B10" s="1">
+        <v>0.28005000000000002</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" s="1">
+        <v>1.40609E+19</v>
+      </c>
+      <c r="B11" s="1">
+        <v>0.35297099999999998</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" s="1">
+        <v>2.92216E+19</v>
+      </c>
+      <c r="B12" s="1">
+        <v>0.49945099999999998</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" s="1">
+        <v>6.49044E+19</v>
+      </c>
+      <c r="B13" s="1">
+        <v>0.60102800000000001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" s="1">
+        <v>3.65744E+20</v>
+      </c>
+      <c r="B14" s="1">
+        <v>0.587279</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" s="1">
+        <v>1.30474E+20</v>
+      </c>
+      <c r="B15" s="1">
+        <v>0.67475399999999996</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB13B395-DD6D-9C4F-8272-CE66807D392F}">
+  <dimension ref="A1:B18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:B18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="1">
+        <v>975371000000000</v>
+      </c>
+      <c r="B2" s="1">
+        <v>4.9370500000000002</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="1">
+        <v>3337840000000000</v>
+      </c>
+      <c r="B3" s="1">
+        <v>5.41587</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
+        <v>6490440000000000</v>
+      </c>
+      <c r="B4" s="1">
+        <v>5.1709199999999997</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
+        <v>1.59282E+16</v>
+      </c>
+      <c r="B5" s="1">
+        <v>5.41587</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
+        <v>4.04109E+16</v>
+      </c>
+      <c r="B6" s="1">
+        <v>6.3682499999999997</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="1">
+        <v>6.02259E+16</v>
+      </c>
+      <c r="B7" s="1">
+        <v>5.0526299999999997</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" s="1">
+        <v>1.86534E+17</v>
+      </c>
+      <c r="B8" s="1">
+        <v>4.3975999999999997</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="1">
+        <v>3.87657E+17</v>
+      </c>
+      <c r="B9" s="1">
+        <v>3.7399399999999998</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" s="1">
+        <v>6.38343E+17</v>
+      </c>
+      <c r="B10" s="1">
+        <v>3.25509</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" s="1">
+        <v>1.56656E+18</v>
+      </c>
+      <c r="B11" s="1">
+        <v>2.2478099999999999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" s="1">
+        <v>3.14916E+18</v>
+      </c>
+      <c r="B12" s="1">
+        <v>2.30043</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" s="1">
+        <v>6.12355E+18</v>
+      </c>
+      <c r="B13" s="1">
+        <v>1.7426299999999999</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" s="1">
+        <v>1.36011E+19</v>
+      </c>
+      <c r="B14" s="1">
+        <v>1.28989</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" s="1">
+        <v>2.92216E+19</v>
+      </c>
+      <c r="B15" s="1">
+        <v>0.95477199999999995</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" s="1">
+        <v>6.07286E+19</v>
+      </c>
+      <c r="B16" s="1">
+        <v>0.74019599999999997</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" s="1">
+        <v>1.30474E+20</v>
+      </c>
+      <c r="B17" s="1">
+        <v>0.65931899999999999</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" s="1">
+        <v>3.7810899999999997E+20</v>
+      </c>
+      <c r="B18" s="1">
+        <v>0.434701</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C3907C3-0FF2-4443-9E86-A13D1E100E09}">
+  <dimension ref="A1:B11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I20" sqref="I20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="1">
+        <v>1042440000000000</v>
+      </c>
+      <c r="B2" s="1">
+        <v>1.7834300000000001E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="1">
+        <v>7.05303E+17</v>
+      </c>
+      <c r="B3" s="1">
+        <v>2.2478100000000001E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
+        <v>1.51532E+18</v>
+      </c>
+      <c r="B4" s="1">
+        <v>1.6638199999999999E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
+        <v>3.04617E+18</v>
+      </c>
+      <c r="B5" s="1">
+        <v>1.6638199999999999E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
+        <v>6.76589E+18</v>
+      </c>
+      <c r="B6" s="1">
+        <v>1.6257600000000001E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="1">
+        <v>1.40609E+19</v>
+      </c>
+      <c r="B7" s="1">
+        <v>1.5522299999999999E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" s="1">
+        <v>3.02096E+19</v>
+      </c>
+      <c r="B8" s="1">
+        <v>1.41499E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="1">
+        <v>6.27818E+19</v>
+      </c>
+      <c r="B9" s="1">
+        <v>1.8251799999999999E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" s="1">
+        <v>1.30474E+20</v>
+      </c>
+      <c r="B10" s="1">
+        <v>1.8679100000000001E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" s="1">
+        <v>3.5378300000000003E+20</v>
+      </c>
+      <c r="B11" s="1">
+        <v>2.0022000000000002E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>